<commit_message>
Modified the data.xlsx file and added new data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRAS\Desktop\excel_express_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB854F8E-F67A-486D-B67A-A52A29EED0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DF150A-89D8-4032-9C42-0165689A5900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7933F2AE-1708-4801-A0BE-65773D240CD6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>edward@example.com</t>
+  </si>
+  <si>
+    <t>Phiri</t>
+  </si>
+  <si>
+    <t>phiri@gmail,com</t>
   </si>
 </sst>
 </file>
@@ -166,13 +172,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15D6D8AC-4C8C-476F-9CC1-DB81ECE379A9}" name="Table2" displayName="Table2" ref="A1:D6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:D6" xr:uid="{15D6D8AC-4C8C-476F-9CC1-DB81ECE379A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15D6D8AC-4C8C-476F-9CC1-DB81ECE379A9}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D7" xr:uid="{15D6D8AC-4C8C-476F-9CC1-DB81ECE379A9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0190CA30-31B9-4C8C-AA9B-E9F48F49B371}" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{14A4DDDB-D21F-4F26-BE53-FF5C32239A5B}" name="NAME" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{CC3010BA-F6D9-4BC5-ABC2-916F531E616E}" name="AGE" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1B77CCFA-3907-4190-BDFE-B0972C9286F7}" name="EMAIL" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{0190CA30-31B9-4C8C-AA9B-E9F48F49B371}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{14A4DDDB-D21F-4F26-BE53-FF5C32239A5B}" name="NAME" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{CC3010BA-F6D9-4BC5-ABC2-916F531E616E}" name="AGE" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1B77CCFA-3907-4190-BDFE-B0972C9286F7}" name="EMAIL" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECB284F-8729-4CD8-91AA-0680F1F58876}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,17 +580,32 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{850830F9-8576-4D86-8301-9A0A56897F39}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{828F24AE-6241-44CC-9BDC-D48D3BB43CA9}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{D7ED524C-DD35-437F-87CD-DFDA2C8AD088}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{E1BC17A9-EBBE-4FA9-95A1-79134CDD9325}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{4D81F4ED-896C-474E-85E3-BD295F31AF59}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{E1BC17A9-EBBE-4FA9-95A1-79134CDD9325}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{D7ED524C-DD35-437F-87CD-DFDA2C8AD088}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{828F24AE-6241-44CC-9BDC-D48D3BB43CA9}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{850830F9-8576-4D86-8301-9A0A56897F39}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{53ABC137-B328-4A5F-B1F2-E8E8209F4EC3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>